<commit_message>
Updated the Transactions functionallity
</commit_message>
<xml_diff>
--- a/DemoDIAPI/Data/Facturas.xlsx
+++ b/DemoDIAPI/Data/Facturas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mvancells\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pfont2\source\repos\DemoDIAPI\DemoDIAPI\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FEACF99-569C-4B9D-96F9-887B66D900ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB8133B-52EC-4C9C-85BD-4D2EF23454AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,79 +31,79 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>CUST009</t>
-  </si>
-  <si>
-    <t>CUST019</t>
-  </si>
-  <si>
-    <t>CUST001</t>
-  </si>
-  <si>
-    <t>CUST005</t>
-  </si>
-  <si>
-    <t>CUST007</t>
-  </si>
-  <si>
-    <t>CUST010</t>
-  </si>
-  <si>
-    <t>CUST014</t>
-  </si>
-  <si>
-    <t>CUST013</t>
-  </si>
-  <si>
-    <t>ITEM0006</t>
-  </si>
-  <si>
-    <t>ITEM0008</t>
-  </si>
-  <si>
-    <t>ITEM0021</t>
-  </si>
-  <si>
-    <t>ITEM0001</t>
-  </si>
-  <si>
-    <t>ITEM0017</t>
-  </si>
-  <si>
-    <t>ITEM0002</t>
-  </si>
-  <si>
-    <t>ITEM0016</t>
-  </si>
-  <si>
-    <t>ITEM0010</t>
-  </si>
-  <si>
-    <t>ITEM0012</t>
-  </si>
-  <si>
-    <t>ITEM0005</t>
-  </si>
-  <si>
-    <t>ITEM0019</t>
-  </si>
-  <si>
-    <t>ITEM0009</t>
-  </si>
-  <si>
-    <t>ITEM0003</t>
-  </si>
-  <si>
-    <t>ITEM0011</t>
-  </si>
-  <si>
-    <t>ITEM0013</t>
-  </si>
-  <si>
-    <t>ITEM0018</t>
-  </si>
-  <si>
-    <t>ITEM0020</t>
+    <t>_CUST001</t>
+  </si>
+  <si>
+    <t>_CUST005</t>
+  </si>
+  <si>
+    <t>_CUST007</t>
+  </si>
+  <si>
+    <t>_CUST009</t>
+  </si>
+  <si>
+    <t>_CUST010</t>
+  </si>
+  <si>
+    <t>_CUST013</t>
+  </si>
+  <si>
+    <t>_CUST014</t>
+  </si>
+  <si>
+    <t>_CUST019</t>
+  </si>
+  <si>
+    <t>_ITEM0001</t>
+  </si>
+  <si>
+    <t>_ITEM0002</t>
+  </si>
+  <si>
+    <t>_ITEM0003</t>
+  </si>
+  <si>
+    <t>_ITEM0005</t>
+  </si>
+  <si>
+    <t>_ITEM0006</t>
+  </si>
+  <si>
+    <t>_ITEM0008</t>
+  </si>
+  <si>
+    <t>_ITEM0009</t>
+  </si>
+  <si>
+    <t>_ITEM0010</t>
+  </si>
+  <si>
+    <t>_ITEM0011</t>
+  </si>
+  <si>
+    <t>_ITEM0012</t>
+  </si>
+  <si>
+    <t>_ITEM0013</t>
+  </si>
+  <si>
+    <t>_ITEM0016</t>
+  </si>
+  <si>
+    <t>_ITEM0017</t>
+  </si>
+  <si>
+    <t>_ITEM0018</t>
+  </si>
+  <si>
+    <t>_ITEM0019</t>
+  </si>
+  <si>
+    <t>_ITEM0020</t>
+  </si>
+  <si>
+    <t>_ITEM0021</t>
   </si>
 </sst>
 </file>
@@ -168,13 +168,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -482,13 +480,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -499,221 +497,221 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>16</v>
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="C3">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>23</v>
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="C4">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>20</v>
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="C5">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>11</v>
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C6">
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>14</v>
+        <v>3</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>12</v>
+        <v>5</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="C8">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>22</v>
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="C9">
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C10">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>24</v>
+        <v>7</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="C11">
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>19</v>
+        <v>7</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="C12">
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>25</v>
+        <v>8</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="C13">
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>14</v>
+      <c r="B14" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="C14">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>16</v>
+      <c r="B15" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="C15">
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>17</v>
+      <c r="B16" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>15</v>
+      <c r="B17" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="C17">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>26</v>
+      <c r="B18" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="C18">
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>21</v>
+        <v>10</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="C19">
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>27</v>
+        <v>10</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="C20">
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="C21">
         <v>68</v>

</xml_diff>

<commit_message>
Fixed UnitPrice from orders
</commit_message>
<xml_diff>
--- a/DemoDIAPI/Data/Facturas.xlsx
+++ b/DemoDIAPI/Data/Facturas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pfont2\source\repos\DemoDIAPI\DemoDIAPI\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB8133B-52EC-4C9C-85BD-4D2EF23454AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1840449F-4E13-4AA5-8E03-D21B326C3440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -480,11 +480,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">

</xml_diff>